<commit_message>
2.4.1 dataset_models refactoring; bugfixes; change default behavior for run scripts
</commit_message>
<xml_diff>
--- a/example_query_file.xlsx
+++ b/example_query_file.xlsx
@@ -1,35 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Le F\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63A52BFE-818F-4039-92EF-9EE92A9A5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6D5B7BAA-0016-4329-88B0-0757EFD005F1}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -39,7 +19,7 @@
     <t>id</t>
   </si>
   <si>
-    <t>question</t>
+    <t>query</t>
   </si>
   <si>
     <t>A</t>
@@ -198,14 +178,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,7 +203,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -228,20 +222,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -252,10 +258,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -282,116 +288,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,408 +375,437 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306E8886-3E5F-4517-999D-016F48AC69DD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="5.88671875" customWidth="1"/>
+    <col min="1" max="1" style="4" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="5.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>